<commit_message>
fix UI and translate to vietnamese
</commit_message>
<xml_diff>
--- a/public/sample_fish_parameters.xlsx.xlsx
+++ b/public/sample_fish_parameters.xlsx.xlsx
@@ -75,7 +75,7 @@
     <t>type</t>
   </si>
   <si>
-    <t>1c46200d-d369-4093-94a6-05d09b4df387</t>
+    <t>2afee2c2-a791-4b50-b73c-2a96bfed943c</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>